<commit_message>
updating XLSX template and adding JSON template
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="261">
   <si>
     <t xml:space="preserve">XRechnung</t>
   </si>
@@ -824,6 +824,9 @@
   </si>
   <si>
     <t xml:space="preserve">application/pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Dateiname der PDF-Datei&gt;</t>
   </si>
 </sst>
 </file>
@@ -1461,7 +1464,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1491,7 +1494,7 @@
   </sheetPr>
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -1523,7 +1526,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="23.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="23.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="n">
         <v>1</v>
       </c>
@@ -1610,7 +1613,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="76.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="77.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
         <v>10</v>
       </c>
@@ -1658,7 +1661,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="173.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="175.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
         <v>20</v>
       </c>
@@ -1688,7 +1691,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="23.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="23.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="16" t="n">
         <v>27</v>
       </c>
@@ -1721,7 +1724,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="23.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="23.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="17" t="n">
         <v>31</v>
       </c>
@@ -1754,7 +1757,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="23.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="23.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="17" t="n">
         <v>34</v>
       </c>
@@ -1769,7 +1772,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="23.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="23.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="17" t="n">
         <v>35</v>
       </c>
@@ -1820,7 +1823,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="23.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="23.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="17" t="n">
         <v>40</v>
       </c>
@@ -1949,7 +1952,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="23.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="23.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="17" t="n">
         <v>50</v>
       </c>
@@ -2000,7 +2003,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="23.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="23.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="17" t="n">
         <v>55</v>
       </c>
@@ -2111,7 +2114,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="23.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="23.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="17" t="n">
         <v>84</v>
       </c>
@@ -2144,7 +2147,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="87.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="88.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="18" t="n">
         <v>86</v>
       </c>
@@ -2291,7 +2294,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="23.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="23.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="n">
         <v>116</v>
       </c>
@@ -2309,7 +2312,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="23.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="23.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="n">
         <v>117</v>
       </c>
@@ -2327,7 +2330,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="119.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="121.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="n">
         <v>118</v>
       </c>
@@ -2360,7 +2363,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="23.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="23.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="22" t="n">
         <v>120</v>
       </c>
@@ -2533,7 +2536,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="76.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="77.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="n">
         <v>130</v>
       </c>
@@ -2548,7 +2551,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="23.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="23.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="n">
         <v>131</v>
       </c>
@@ -2596,7 +2599,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="23.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="23.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="n">
         <v>146</v>
       </c>
@@ -2614,7 +2617,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="119.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="121.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="n">
         <v>151</v>
       </c>
@@ -2704,10 +2707,10 @@
   </sheetPr>
   <dimension ref="A1:XFD42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2780,7 +2783,7 @@
       </c>
       <c r="D3" s="40" t="n">
         <f aca="true">TODAY()</f>
-        <v>45671</v>
+        <v>45680</v>
       </c>
       <c r="E3" s="41" t="str">
         <f aca="false">VLOOKUP($A3,BusinessTerms!$A:$D,4,0)</f>
@@ -2847,7 +2850,7 @@
       </c>
       <c r="D6" s="40" t="n">
         <f aca="true">TODAY()+7</f>
-        <v>45678</v>
+        <v>45687</v>
       </c>
       <c r="E6" s="41" t="str">
         <f aca="false">VLOOKUP($A6,BusinessTerms!$A:$D,4,0)</f>
@@ -3436,7 +3439,7 @@
       </c>
       <c r="D35" s="48" t="n">
         <f aca="true">TODAY()-14</f>
-        <v>45657</v>
+        <v>45666</v>
       </c>
       <c r="E35" s="43" t="str">
         <f aca="false">VLOOKUP($A35,BusinessTerms!$A:$D,4,0)</f>
@@ -3461,7 +3464,7 @@
       </c>
       <c r="D36" s="40" t="n">
         <f aca="true">TODAY()-7</f>
-        <v>45664</v>
+        <v>45673</v>
       </c>
       <c r="E36" s="45" t="str">
         <f aca="false">VLOOKUP($A36,BusinessTerms!$A:$D,4,0)</f>
@@ -3562,7 +3565,9 @@
         <f aca="false">VLOOKUP($A41,BusinessTerms!$A:$D,3,0)</f>
         <v>0</v>
       </c>
-      <c r="D41" s="47"/>
+      <c r="D41" s="47" t="n">
+        <v>0</v>
+      </c>
       <c r="E41" s="45" t="str">
         <f aca="false">VLOOKUP($A41,BusinessTerms!$A:$D,4,0)</f>
         <v>Vorauszahlungsbetrag</v>
@@ -3621,7 +3626,7 @@
   </sheetPr>
   <dimension ref="A1:XFD12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
@@ -3822,7 +3827,7 @@
       </c>
       <c r="D6" s="40" t="n">
         <f aca="true">TODAY()-14</f>
-        <v>45657</v>
+        <v>45666</v>
       </c>
       <c r="E6" s="57"/>
       <c r="F6" s="57"/>
@@ -3847,7 +3852,7 @@
       </c>
       <c r="D7" s="40" t="n">
         <f aca="true">TODAY()-7</f>
-        <v>45664</v>
+        <v>45673</v>
       </c>
       <c r="E7" s="57"/>
       <c r="F7" s="57"/>
@@ -4032,7 +4037,7 @@
   </sheetPr>
   <dimension ref="A1:XFD6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -4116,7 +4121,7 @@
         <v>Kennung der rechnungsbegründenden Unterlage</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="23.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="23.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <v>123</v>
       </c>
@@ -4206,7 +4211,9 @@
         <f aca="false">VLOOKUP($A6,BusinessTerms!$A:$D,3,0)</f>
         <v>1</v>
       </c>
-      <c r="D6" s="62"/>
+      <c r="D6" s="62" t="s">
+        <v>260</v>
+      </c>
       <c r="E6" s="62"/>
       <c r="F6" s="62"/>
       <c r="G6" s="62"/>

</xml_diff>

<commit_message>
added MIME code for spreadsheet invoice attachments
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -826,7 +826,7 @@
     <t xml:space="preserve">application/pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;Dateiname der PDF-Datei&gt;</t>
+    <t xml:space="preserve">&lt;Dateinamei&gt;</t>
   </si>
 </sst>
 </file>
@@ -1464,7 +1464,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1494,7 +1494,7 @@
   </sheetPr>
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -1613,7 +1613,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="77.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="76.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
         <v>10</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="175.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="173.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
         <v>20</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="88.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="87.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="18" t="n">
         <v>86</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="121.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="119.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="n">
         <v>118</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="77.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="76.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="n">
         <v>130</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="121.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="119.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="n">
         <v>151</v>
       </c>
@@ -2707,10 +2707,10 @@
   </sheetPr>
   <dimension ref="A1:XFD42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2783,7 +2783,7 @@
       </c>
       <c r="D3" s="40" t="n">
         <f aca="true">TODAY()</f>
-        <v>45680</v>
+        <v>45690</v>
       </c>
       <c r="E3" s="41" t="str">
         <f aca="false">VLOOKUP($A3,BusinessTerms!$A:$D,4,0)</f>
@@ -2850,7 +2850,7 @@
       </c>
       <c r="D6" s="40" t="n">
         <f aca="true">TODAY()+7</f>
-        <v>45687</v>
+        <v>45697</v>
       </c>
       <c r="E6" s="41" t="str">
         <f aca="false">VLOOKUP($A6,BusinessTerms!$A:$D,4,0)</f>
@@ -3439,7 +3439,7 @@
       </c>
       <c r="D35" s="48" t="n">
         <f aca="true">TODAY()-14</f>
-        <v>45666</v>
+        <v>45676</v>
       </c>
       <c r="E35" s="43" t="str">
         <f aca="false">VLOOKUP($A35,BusinessTerms!$A:$D,4,0)</f>
@@ -3464,7 +3464,7 @@
       </c>
       <c r="D36" s="40" t="n">
         <f aca="true">TODAY()-7</f>
-        <v>45673</v>
+        <v>45683</v>
       </c>
       <c r="E36" s="45" t="str">
         <f aca="false">VLOOKUP($A36,BusinessTerms!$A:$D,4,0)</f>
@@ -3626,7 +3626,7 @@
   </sheetPr>
   <dimension ref="A1:XFD12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
@@ -3827,7 +3827,7 @@
       </c>
       <c r="D6" s="40" t="n">
         <f aca="true">TODAY()-14</f>
-        <v>45666</v>
+        <v>45676</v>
       </c>
       <c r="E6" s="57"/>
       <c r="F6" s="57"/>
@@ -3852,7 +3852,7 @@
       </c>
       <c r="D7" s="40" t="n">
         <f aca="true">TODAY()-7</f>
-        <v>45673</v>
+        <v>45683</v>
       </c>
       <c r="E7" s="57"/>
       <c r="F7" s="57"/>
@@ -4037,7 +4037,7 @@
   </sheetPr>
   <dimension ref="A1:XFD6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -4179,19 +4179,19 @@
         <f aca="false">VLOOKUP($A5,BusinessTerms!$A:$D,3,0)</f>
         <v>1</v>
       </c>
-      <c r="D5" s="56" t="s">
+      <c r="D5" s="55" t="s">
         <v>259</v>
       </c>
-      <c r="E5" s="56" t="s">
+      <c r="E5" s="55" t="s">
         <v>259</v>
       </c>
-      <c r="F5" s="56" t="s">
+      <c r="F5" s="55" t="s">
         <v>259</v>
       </c>
-      <c r="G5" s="56" t="s">
+      <c r="G5" s="55" t="s">
         <v>259</v>
       </c>
-      <c r="H5" s="56" t="s">
+      <c r="H5" s="55" t="s">
         <v>259</v>
       </c>
       <c r="I5" s="53" t="str">
@@ -4230,6 +4230,12 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D5:H5" type="list">
+      <formula1>"application/pdf,application/vnd.openxmlformats-officedocument.spreadsheetml.sheet"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>